<commit_message>
[KadabraAst] Updates sheet with study of AST nodes to implement
</commit_message>
<xml_diff>
--- a/KadabraAst/AST Nodes To Implement.xlsx
+++ b/KadabraAst/AST Nodes To Implement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="73">
   <si>
     <t>Node</t>
   </si>
@@ -174,15 +174,9 @@
     <t>YieldStmt</t>
   </si>
   <si>
-    <t>VariableAccess</t>
-  </si>
-  <si>
     <t>Expression</t>
   </si>
   <si>
-    <t>FieldAccess</t>
-  </si>
-  <si>
     <t>ArrayAccess</t>
   </si>
   <si>
@@ -229,13 +223,28 @@
   </si>
   <si>
     <t>CommentStmt</t>
+  </si>
+  <si>
+    <t>Partially based on:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.oracle.com/javase/specs/jls/se17/html/jls-19.html </t>
+  </si>
+  <si>
+    <t>CaseStmt</t>
+  </si>
+  <si>
+    <t>DeclReference</t>
+  </si>
+  <si>
+    <t>Annotation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +267,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -276,16 +293,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -565,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +598,7 @@
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -603,14 +623,17 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="2">
-        <f>COUNTA(F:F)/COUNTA(A2:A57)</f>
+        <f>COUNTA(F:F)/COUNTA(A2:A56)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -618,10 +641,13 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -629,10 +655,10 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -640,10 +666,10 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -651,117 +677,117 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>52</v>
-      </c>
-      <c r="F8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,7 +798,7 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -783,7 +809,7 @@
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,29 +820,29 @@
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -827,18 +853,18 @@
         <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -852,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,7 +892,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -877,7 +903,7 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -888,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,7 +925,7 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -910,45 +936,45 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -957,7 +983,7 @@
         <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -968,7 +994,7 @@
         <v>21</v>
       </c>
       <c r="F34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -979,7 +1005,7 @@
         <v>21</v>
       </c>
       <c r="F35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,7 +1016,7 @@
         <v>21</v>
       </c>
       <c r="F36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,7 +1027,7 @@
         <v>21</v>
       </c>
       <c r="F37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,7 +1038,7 @@
         <v>21</v>
       </c>
       <c r="F38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,7 +1049,7 @@
         <v>21</v>
       </c>
       <c r="F39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1034,7 +1060,7 @@
         <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1045,7 +1071,7 @@
         <v>38</v>
       </c>
       <c r="F41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1056,7 +1082,7 @@
         <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1067,7 +1093,7 @@
         <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,7 +1104,7 @@
         <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1089,7 +1115,7 @@
         <v>38</v>
       </c>
       <c r="F45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,7 +1126,7 @@
         <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,7 +1137,7 @@
         <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1122,7 +1148,7 @@
         <v>21</v>
       </c>
       <c r="F48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1133,7 +1159,7 @@
         <v>21</v>
       </c>
       <c r="F49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1144,7 +1170,7 @@
         <v>21</v>
       </c>
       <c r="F50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1155,7 +1181,7 @@
         <v>21</v>
       </c>
       <c r="F51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1166,7 +1192,7 @@
         <v>23</v>
       </c>
       <c r="F52" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1177,7 +1203,7 @@
         <v>23</v>
       </c>
       <c r="F53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1194,7 +1220,7 @@
         <v>18</v>
       </c>
       <c r="F54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,7 +1231,7 @@
         <v>7</v>
       </c>
       <c r="F55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1216,41 +1242,49 @@
         <v>30</v>
       </c>
       <c r="F56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
-        <v>51</v>
-      </c>
-      <c r="F57" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D58" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:E56">
     <sortCondition ref="D2:D56"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[KadabraAst] Updates planning Excel
</commit_message>
<xml_diff>
--- a/KadabraAst/AST Nodes To Implement.xlsx
+++ b/KadabraAst/AST Nodes To Implement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
   <si>
     <t>Node</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Generating Code</t>
   </si>
   <si>
-    <t>Cleared TODOs</t>
-  </si>
-  <si>
     <t>Only elements that can be referenced should be Decl</t>
   </si>
   <si>
@@ -250,6 +247,21 @@
   </si>
   <si>
     <t>Package</t>
+  </si>
+  <si>
+    <t>Parsing</t>
+  </si>
+  <si>
+    <t>CtMethod</t>
+  </si>
+  <si>
+    <t>CtInvocationImpl</t>
+  </si>
+  <si>
+    <t>TypeAccess</t>
+  </si>
+  <si>
+    <t>CtTypeAccess</t>
   </si>
 </sst>
 </file>
@@ -597,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +641,7 @@
         <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>72</v>
@@ -652,8 +664,8 @@
         <v>60</v>
       </c>
       <c r="K2" s="2">
-        <f>COUNTA(I:I)/COUNTA(A2:A55)</f>
-        <v>1.0185185185185186</v>
+        <f>COUNTA(I:I)/COUNTA(A2:A56)</f>
+        <v>1</v>
       </c>
       <c r="L2" t="s">
         <v>64</v>
@@ -675,7 +687,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -686,7 +698,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -741,18 +753,21 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="I10" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
@@ -763,7 +778,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -774,7 +789,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -785,7 +800,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
@@ -796,7 +811,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
@@ -807,13 +822,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="I16" t="s">
         <v>60</v>
@@ -821,71 +833,74 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
       <c r="I17" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
       <c r="I18" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
       <c r="I19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
       <c r="I20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
       <c r="I21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I22" t="s">
         <v>60</v>
@@ -893,13 +908,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I23" t="s">
         <v>60</v>
@@ -907,13 +919,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I24" t="s">
         <v>60</v>
@@ -921,7 +933,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -932,18 +947,24 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
       <c r="I26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -954,7 +975,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -965,10 +986,10 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="I29" t="s">
         <v>60</v>
@@ -976,7 +997,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
         <v>54</v>
@@ -987,7 +1008,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
         <v>54</v>
@@ -998,13 +1019,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="I32" t="s">
         <v>60</v>
@@ -1012,10 +1030,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
       </c>
       <c r="D33" t="s">
         <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>60</v>
       </c>
       <c r="I33" t="s">
         <v>60</v>
@@ -1023,7 +1047,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
         <v>19</v>
@@ -1034,7 +1058,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
@@ -1045,7 +1069,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
@@ -1056,7 +1080,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
@@ -1067,7 +1091,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
@@ -1078,10 +1102,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I39" t="s">
         <v>60</v>
@@ -1089,7 +1113,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
         <v>35</v>
@@ -1100,10 +1124,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I41" t="s">
         <v>60</v>
@@ -1111,7 +1135,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
         <v>19</v>
@@ -1122,7 +1146,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
         <v>19</v>
@@ -1133,10 +1157,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I44" t="s">
         <v>60</v>
@@ -1144,10 +1168,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I45" t="s">
         <v>60</v>
@@ -1155,7 +1179,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
         <v>19</v>
@@ -1166,7 +1190,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -1177,7 +1201,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
         <v>19</v>
@@ -1188,7 +1212,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D49" t="s">
         <v>19</v>
@@ -1199,7 +1223,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" t="s">
         <v>19</v>
@@ -1210,10 +1234,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D51" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I51" t="s">
         <v>60</v>
@@ -1221,7 +1245,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D52" t="s">
         <v>21</v>
@@ -1232,16 +1256,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I53" t="s">
         <v>60</v>
@@ -1249,21 +1267,33 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
       </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" t="s">
+        <v>60</v>
+      </c>
+      <c r="H54" t="s">
+        <v>17</v>
+      </c>
       <c r="I54" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="I55" t="s">
         <v>60</v>
@@ -1271,23 +1301,26 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="I56" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D58" t="s">
         <v>19</v>
@@ -1295,10 +1328,18 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>68</v>
       </c>
-      <c r="D59" t="s">
-        <v>48</v>
+      <c r="D60" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[KadabraAst] Adds LocalVarDecl.IS_INFERRED and updates excel
</commit_message>
<xml_diff>
--- a/KadabraAst/AST Nodes To Implement.xlsx
+++ b/KadabraAst/AST Nodes To Implement.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="84">
   <si>
     <t>Node</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>CtTypeAccess</t>
+  </si>
+  <si>
+    <t>CtLocalVariableImpl</t>
+  </si>
+  <si>
+    <t>CtExpression</t>
+  </si>
+  <si>
+    <t>CtLiteral</t>
   </si>
 </sst>
 </file>
@@ -611,20 +620,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +662,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -671,7 +680,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -685,7 +694,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -696,7 +705,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -707,7 +716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -718,10 +727,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
@@ -729,7 +741,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -740,7 +752,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -751,7 +763,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -762,7 +774,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -776,7 +788,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -787,7 +799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -798,7 +810,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -809,7 +821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -820,7 +832,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -831,7 +843,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -845,7 +857,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -856,7 +868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -870,18 +882,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
       <c r="D20" t="s">
         <v>18</v>
       </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
       <c r="I20" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -895,7 +913,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -906,7 +924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -917,7 +935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -931,7 +949,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -945,7 +963,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -962,7 +980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -973,10 +991,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
@@ -984,18 +1005,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="I29" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1006,7 +1027,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1017,7 +1038,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -1028,7 +1049,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1045,7 +1066,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1056,7 +1077,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1067,7 +1088,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1078,7 +1099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1089,7 +1110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -1100,7 +1121,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -1111,7 +1132,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1122,7 +1143,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -1133,7 +1154,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -1144,7 +1165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1155,7 +1176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -1166,7 +1187,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -1177,7 +1198,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1188,7 +1209,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -1199,7 +1220,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -1210,7 +1231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -1221,7 +1242,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -1232,7 +1253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -1243,7 +1264,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -1254,7 +1275,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -1265,7 +1286,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>9</v>
       </c>
@@ -1288,7 +1309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -1299,7 +1320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -1310,7 +1331,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -1318,7 +1339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -1326,7 +1347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -1334,7 +1355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>68</v>
       </c>

</xml_diff>